<commit_message>
FIX[Calc]: Imports tables with no headers properly (#304)
</commit_message>
<xml_diff>
--- a/packages/calc/equalto_xlsx/tests/calc_test_no_export/tables.xlsx
+++ b/packages/calc/equalto_xlsx/tests/calc_test_no_export/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Library/CloudStorage/Dropbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2FA1B4-1920-B744-87E6-31D15CAC84E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2DDAA2-CD5A-7244-974F-D266763ECB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="2460" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{234D3629-A973-D04E-93AE-20E06D5B5DDB}"/>
+    <workbookView xWindow="4200" yWindow="2460" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{234D3629-A973-D04E-93AE-20E06D5B5DDB}"/>
   </bookViews>
   <sheets>
     <sheet name="WithHeaders" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="filters" sheetId="4" r:id="rId4"/>
     <sheet name="Functions Filters" sheetId="5" r:id="rId5"/>
     <sheet name="Functions Hidden" sheetId="6" r:id="rId6"/>
+    <sheet name="No Headers" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="62">
   <si>
     <t>Jan</t>
   </si>
@@ -221,6 +222,12 @@
   </si>
   <si>
     <t>NOTE FOR A TEST: Hidde column 3 for table in the left but filtered for table in the right</t>
+  </si>
+  <si>
+    <t>"Hope" is the thing without Headers.. that perches in the soul, and sings the tune without the words. And never stops... at all</t>
+  </si>
+  <si>
+    <t>No Headers, no cry</t>
   </si>
 </sst>
 </file>
@@ -356,28 +363,28 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -386,22 +393,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -409,7 +416,10 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -437,167 +447,6 @@
         </top>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="7"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -650,6 +499,34 @@
       </font>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -661,6 +538,33 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -712,6 +616,33 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -723,6 +654,33 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -774,6 +732,33 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -796,13 +781,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="7" tint="0.39997558519241921"/>
         </left>
@@ -818,7 +796,36 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="7"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -849,6 +856,9 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -893,9 +903,6 @@
       <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -920,6 +927,9 @@
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -948,7 +958,7 @@
     </tableColumn>
     <tableColumn id="4" xr3:uid="{EAB60CA7-224E-E148-A760-EB424EB2A193}" name="Apr" totalsRowFunction="sum"/>
     <tableColumn id="5" xr3:uid="{B522D1CB-9A2C-634E-BDD7-B62903431D77}" name="Dec" totalsRowFunction="sum"/>
-    <tableColumn id="6" xr3:uid="{EA41A6B3-90DE-8243-83DD-288BE6A6D399}" name="Year" totalsRowFunction="sum" dataDxfId="27">
+    <tableColumn id="6" xr3:uid="{EA41A6B3-90DE-8243-83DD-288BE6A6D399}" name="Year" totalsRowFunction="sum" dataDxfId="28">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[Jan]:[Dec]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1010,8 +1020,8 @@
     <tableColumn id="3" xr3:uid="{008FD32A-29F7-574E-A3CA-DFEEBFC2BC83}" name="Rep"/>
     <tableColumn id="4" xr3:uid="{51EC3971-83D9-F544-A07E-B9742F61E585}" name="Item"/>
     <tableColumn id="5" xr3:uid="{45346D50-C4CC-AE4B-9A8F-3E9CB08991CE}" name="Units" totalsRowFunction="average"/>
-    <tableColumn id="6" xr3:uid="{D5FD35D4-3304-2241-A051-BEE9DE9C975E}" name="Unit Cost" totalsRowFunction="average" totalsRowDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{B4609346-B08C-1540-87A6-7BDD0F99D755}" name="Total" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="24" dataCellStyle="Comma">
+    <tableColumn id="6" xr3:uid="{D5FD35D4-3304-2241-A051-BEE9DE9C975E}" name="Unit Cost" totalsRowFunction="average" totalsRowDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{B4609346-B08C-1540-87A6-7BDD0F99D755}" name="Total" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Comma">
       <calculatedColumnFormula>Table16[[#This Row],[Units]]*Table16[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1021,14 +1031,34 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{49AA31D8-9444-7542-AA9B-6F1C2E72E16D}" name="Table17" displayName="Table17" ref="A1:F45" totalsRowCount="1">
-  <autoFilter ref="A1:F44" xr:uid="{49AA31D8-9444-7542-AA9B-6F1C2E72E16D}"/>
+  <autoFilter ref="A1:F44" xr:uid="{49AA31D8-9444-7542-AA9B-6F1C2E72E16D}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Andres"/>
+        <filter val="Diarmuid"/>
+        <filter val="Howard"/>
+        <filter val="Ivan"/>
+        <filter val="Ken"/>
+        <filter val="Lowel"/>
+        <filter val="Mira"/>
+        <filter val="Parent"/>
+        <filter val="Town"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="greaterThanOrEqual" val="20"/>
+        <customFilter operator="notEqual" val="22"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{833D4BD4-E79F-5F42-8F2A-C9BE7C363401}" name="Region" totalsRowLabel="Total" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{6D8BA91D-5F28-094A-B6F3-A121A3AD338E}" name="Rep" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{79351C90-216B-6644-95CF-452CE101F1D2}" name="Item" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{08B2CDA5-31A0-154D-A4DB-93A805099430}" name="Units" totalsRowFunction="min" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{3ECC1DE3-3552-C54E-9514-43BA9F5B787E}" name="Unit Cost" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="17" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{E116183D-D911-3044-B68F-51A37E321D80}" name="Total" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="16" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{833D4BD4-E79F-5F42-8F2A-C9BE7C363401}" name="Region" totalsRowLabel="Total" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{6D8BA91D-5F28-094A-B6F3-A121A3AD338E}" name="Rep" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{79351C90-216B-6644-95CF-452CE101F1D2}" name="Item" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{08B2CDA5-31A0-154D-A4DB-93A805099430}" name="Units" totalsRowFunction="min" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{3ECC1DE3-3552-C54E-9514-43BA9F5B787E}" name="Unit Cost" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{E116183D-D911-3044-B68F-51A37E321D80}" name="Total" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Comma">
       <calculatedColumnFormula>Table17[[#This Row],[Units]]*Table17[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1037,19 +1067,36 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2FB4BD79-54FB-7D43-BEEE-37F9A827C0DE}" name="Table7" displayName="Table7" ref="J1:O8" totalsRowCount="1" headerRowDxfId="6" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2FB4BD79-54FB-7D43-BEEE-37F9A827C0DE}" name="Table7" displayName="Table7" ref="J1:O8" totalsRowCount="1" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="J1:O7" xr:uid="{2FB4BD79-54FB-7D43-BEEE-37F9A827C0DE}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5FF2180F-76F9-A746-8C55-BBB6F0393834}" name="Region" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D0548A0A-1672-894E-BCDE-D702C6719251}" name="Rep" dataDxfId="11" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{2AF4D54E-D49C-BA48-AAC6-F8060165BB28}" name="Item" dataDxfId="10" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{4DDC914F-CC98-0B4A-98C6-EA049121457C}" name="Units" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{E99A81FC-8139-C141-9352-61D048323D3C}" name="Unit Cost" totalsRowFunction="average" dataDxfId="8" totalsRowDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{75303A0A-2CA3-FC45-B09C-7BEF7FE97225}" name="Total" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="0" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{5FF2180F-76F9-A746-8C55-BBB6F0393834}" name="Region" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{D0548A0A-1672-894E-BCDE-D702C6719251}" name="Rep" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{2AF4D54E-D49C-BA48-AAC6-F8060165BB28}" name="Item" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{4DDC914F-CC98-0B4A-98C6-EA049121457C}" name="Units" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{E99A81FC-8139-C141-9352-61D048323D3C}" name="Unit Cost" totalsRowFunction="average" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{75303A0A-2CA3-FC45-B09C-7BEF7FE97225}" name="Total" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Comma">
       <calculatedColumnFormula>Table17[[#This Row],[Units]]*Table17[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{189316EE-C132-0C45-AF12-4398914EC685}" name="Table8" displayName="Table8" ref="B3:F8" headerRowCount="0" totalsRowCount="1">
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{FD12ED3A-517C-074D-85FE-8C4DF0F29F65}" name="Column1" totalsRowFunction="min"/>
+    <tableColumn id="2" xr3:uid="{C9107CA1-9D11-1F48-BD7F-AF34A7BD44B3}" name="Column2" totalsRowFunction="sum"/>
+    <tableColumn id="3" xr3:uid="{D2AF1492-6468-5243-94F7-814F63BA6038}" name="Column3" totalsRowFunction="custom">
+      <totalsRowFormula>SUBTOTAL(9,Table8[Column3])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{DEF2B5E7-1C88-E94A-979A-299DB49B58E3}" name="Column4" totalsRowFunction="sum"/>
+    <tableColumn id="5" xr3:uid="{646CE8D4-3EDF-604D-BB6D-74D5208E9A47}" name="Column5" totalsRowFunction="average" dataDxfId="0">
+      <calculatedColumnFormula>Table8[[#This Row],[Column1]]*Table8[[#This Row],[Column2]]+Table8[[#This Row],[Column3]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2935,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C59673F-08B4-F543-8A6A-D28D5C3CA8E0}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3223,7 +3270,7 @@
         <v>224.55</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -3420,7 +3467,7 @@
         <v>174.65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
@@ -3444,7 +3491,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -3465,7 +3512,7 @@
         <v>255.84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
@@ -3486,7 +3533,7 @@
         <v>251.72</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
@@ -3508,7 +3555,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>46</v>
       </c>
@@ -3529,7 +3576,7 @@
         <v>299.84999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -3613,7 +3660,7 @@
         <v>413.54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
@@ -3718,7 +3765,7 @@
         <v>131.34</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
@@ -3739,7 +3786,7 @@
         <v>479.04</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>48</v>
       </c>
@@ -3760,7 +3807,7 @@
         <v>68.37</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>48</v>
       </c>
@@ -3781,7 +3828,7 @@
         <v>719.2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>48</v>
       </c>
@@ -3802,7 +3849,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>46</v>
       </c>
@@ -3949,7 +3996,7 @@
         <v>1139.4299999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>48</v>
       </c>
@@ -4012,7 +4059,7 @@
         <v>1879.06</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -4037,17 +4084,17 @@
       <c r="A45" t="s">
         <v>6</v>
       </c>
-      <c r="D45">
+      <c r="D45" t="e">
         <f>SUBTOTAL(105,Table17[Units])</f>
-        <v>0.5</v>
+        <v>#N/A</v>
       </c>
       <c r="E45" s="8">
         <f>SUBTOTAL(109,Table17[Unit Cost])</f>
-        <v>665.78</v>
-      </c>
-      <c r="F45" s="8">
+        <v>721.72</v>
+      </c>
+      <c r="F45" s="8" t="e">
         <f>SUBTOTAL(109,Table17[Total])</f>
-        <v>14660.684999999998</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -4057,20 +4104,20 @@
       </c>
       <c r="E46">
         <f>SUBTOTAL(9,Table17[Unit Cost])</f>
-        <v>873.2700000000001</v>
+        <v>721.72</v>
       </c>
       <c r="G46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D47">
+      <c r="D47" t="e">
         <f>SUBTOTAL(109, Table17[Units])</f>
-        <v>1224.5</v>
-      </c>
-      <c r="E47">
+        <v>#N/A</v>
+      </c>
+      <c r="E47" t="e">
         <f>SUBTOTAL(105,Table17[Units])</f>
-        <v>0.5</v>
+        <v>#N/A</v>
       </c>
       <c r="G47" t="s">
         <v>37</v>
@@ -4086,9 +4133,9 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D49">
+      <c r="D49" t="e">
         <f>SUBTOTAL(101.2,Table17[Units])</f>
-        <v>42.224137931034484</v>
+        <v>#N/A</v>
       </c>
       <c r="G49" t="s">
         <v>58</v>
@@ -4097,13 +4144,13 @@
     <row r="51" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E51">
         <f>SUBTOTAL(6,Table17[Unit Cost])</f>
-        <v>4.5253473053046947E+37</v>
+        <v>7.3394670378456595E+32</v>
       </c>
     </row>
     <row r="52" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E52">
         <f>SUBTOTAL(106, Table17[Unit Cost])</f>
-        <v>3.78850125560893E+27</v>
+        <v>7.3394670378456595E+32</v>
       </c>
     </row>
   </sheetData>
@@ -4113,4 +4160,145 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B23473F-5DA6-0940-893D-89F02152A971}">
+  <dimension ref="B2:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <f>Table8[[#This Row],[Column1]]*Table8[[#This Row],[Column2]]+Table8[[#This Row],[Column3]]</f>
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>89</v>
+      </c>
+      <c r="F4">
+        <f>Table8[[#This Row],[Column1]]*Table8[[#This Row],[Column2]]+Table8[[#This Row],[Column3]]</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f>Table8[[#This Row],[Column1]]*Table8[[#This Row],[Column2]]+Table8[[#This Row],[Column3]]</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>123</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f>Table8[[#This Row],[Column1]]*Table8[[#This Row],[Column2]]+Table8[[#This Row],[Column3]]</f>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <f>Table8[[#This Row],[Column1]]*Table8[[#This Row],[Column2]]+Table8[[#This Row],[Column3]]</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>SUBTOTAL(105,Table8[Column1])</f>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f>SUBTOTAL(109,Table8[Column2])</f>
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <f>SUBTOTAL(9,Table8[Column3])</f>
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <f>SUBTOTAL(109,Table8[Column4])</f>
+        <v>98</v>
+      </c>
+      <c r="F8">
+        <f>SUBTOTAL(101,Table8[Column5])</f>
+        <v>112.4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <f>SUM(Table8[#Data])</f>
+        <v>853</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATE[tables]: Escapes column names properly (#310)
Adds all SUBTOTAL functions
</commit_message>
<xml_diff>
--- a/packages/calc/equalto_xlsx/tests/calc_test_no_export/tables.xlsx
+++ b/packages/calc/equalto_xlsx/tests/calc_test_no_export/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Library/CloudStorage/Dropbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2DDAA2-CD5A-7244-974F-D266763ECB47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C75E367-1D12-644E-9BDE-F8C50425E666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="2460" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{234D3629-A973-D04E-93AE-20E06D5B5DDB}"/>
+    <workbookView xWindow="4200" yWindow="2460" windowWidth="28040" windowHeight="17440" activeTab="7" xr2:uid="{234D3629-A973-D04E-93AE-20E06D5B5DDB}"/>
   </bookViews>
   <sheets>
     <sheet name="WithHeaders" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Functions Filters" sheetId="5" r:id="rId5"/>
     <sheet name="Functions Hidden" sheetId="6" r:id="rId6"/>
     <sheet name="No Headers" sheetId="7" r:id="rId7"/>
+    <sheet name="Escape" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="69">
   <si>
     <t>Jan</t>
   </si>
@@ -228,6 +229,27 @@
   </si>
   <si>
     <t>No Headers, no cry</t>
+  </si>
+  <si>
+    <t>#Shame</t>
+  </si>
+  <si>
+    <t>[Not me]</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Totals []^&amp;*@#$,,&lt;&gt;</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Hi, 'This</t>
   </si>
 </sst>
 </file>
@@ -416,7 +438,10 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="30">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -958,7 +983,7 @@
     </tableColumn>
     <tableColumn id="4" xr3:uid="{EAB60CA7-224E-E148-A760-EB424EB2A193}" name="Apr" totalsRowFunction="sum"/>
     <tableColumn id="5" xr3:uid="{B522D1CB-9A2C-634E-BDD7-B62903431D77}" name="Dec" totalsRowFunction="sum"/>
-    <tableColumn id="6" xr3:uid="{EA41A6B3-90DE-8243-83DD-288BE6A6D399}" name="Year" totalsRowFunction="sum" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{EA41A6B3-90DE-8243-83DD-288BE6A6D399}" name="Year" totalsRowFunction="sum" dataDxfId="29">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[Jan]:[Dec]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1014,14 +1039,21 @@
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{27E1DFED-3E48-FA46-A70C-AD40366253C9}" name="Table16" displayName="Table16" ref="A1:F45" totalsRowCount="1">
-  <autoFilter ref="A1:F44" xr:uid="{27E1DFED-3E48-FA46-A70C-AD40366253C9}"/>
+  <autoFilter ref="A1:F44" xr:uid="{27E1DFED-3E48-FA46-A70C-AD40366253C9}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Germany"/>
+        <filter val="Spain"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{395CBC8A-3FD4-8E49-9460-D39176107019}" name="Region"/>
     <tableColumn id="3" xr3:uid="{008FD32A-29F7-574E-A3CA-DFEEBFC2BC83}" name="Rep"/>
     <tableColumn id="4" xr3:uid="{51EC3971-83D9-F544-A07E-B9742F61E585}" name="Item"/>
     <tableColumn id="5" xr3:uid="{45346D50-C4CC-AE4B-9A8F-3E9CB08991CE}" name="Units" totalsRowFunction="average"/>
-    <tableColumn id="6" xr3:uid="{D5FD35D4-3304-2241-A051-BEE9DE9C975E}" name="Unit Cost" totalsRowFunction="average" totalsRowDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{B4609346-B08C-1540-87A6-7BDD0F99D755}" name="Total" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Comma">
+    <tableColumn id="6" xr3:uid="{D5FD35D4-3304-2241-A051-BEE9DE9C975E}" name="Unit Cost" totalsRowFunction="average" totalsRowDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{B4609346-B08C-1540-87A6-7BDD0F99D755}" name="Total" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26" dataCellStyle="Comma">
       <calculatedColumnFormula>Table16[[#This Row],[Units]]*Table16[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1031,34 +1063,14 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{49AA31D8-9444-7542-AA9B-6F1C2E72E16D}" name="Table17" displayName="Table17" ref="A1:F45" totalsRowCount="1">
-  <autoFilter ref="A1:F44" xr:uid="{49AA31D8-9444-7542-AA9B-6F1C2E72E16D}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Andres"/>
-        <filter val="Diarmuid"/>
-        <filter val="Howard"/>
-        <filter val="Ivan"/>
-        <filter val="Ken"/>
-        <filter val="Lowel"/>
-        <filter val="Mira"/>
-        <filter val="Parent"/>
-        <filter val="Town"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <customFilters>
-        <customFilter operator="greaterThanOrEqual" val="20"/>
-        <customFilter operator="notEqual" val="22"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F44" xr:uid="{49AA31D8-9444-7542-AA9B-6F1C2E72E16D}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{833D4BD4-E79F-5F42-8F2A-C9BE7C363401}" name="Region" totalsRowLabel="Total" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{6D8BA91D-5F28-094A-B6F3-A121A3AD338E}" name="Rep" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{79351C90-216B-6644-95CF-452CE101F1D2}" name="Item" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{08B2CDA5-31A0-154D-A4DB-93A805099430}" name="Units" totalsRowFunction="min" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{3ECC1DE3-3552-C54E-9514-43BA9F5B787E}" name="Unit Cost" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{E116183D-D911-3044-B68F-51A37E321D80}" name="Total" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{833D4BD4-E79F-5F42-8F2A-C9BE7C363401}" name="Region" totalsRowLabel="Total" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{6D8BA91D-5F28-094A-B6F3-A121A3AD338E}" name="Rep" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{79351C90-216B-6644-95CF-452CE101F1D2}" name="Item" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{08B2CDA5-31A0-154D-A4DB-93A805099430}" name="Units" totalsRowFunction="min" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{3ECC1DE3-3552-C54E-9514-43BA9F5B787E}" name="Unit Cost" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{E116183D-D911-3044-B68F-51A37E321D80}" name="Total" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Comma">
       <calculatedColumnFormula>Table17[[#This Row],[Units]]*Table17[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1067,15 +1079,15 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2FB4BD79-54FB-7D43-BEEE-37F9A827C0DE}" name="Table7" displayName="Table7" ref="J1:O8" totalsRowCount="1" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{2FB4BD79-54FB-7D43-BEEE-37F9A827C0DE}" name="Table7" displayName="Table7" ref="J1:O8" totalsRowCount="1" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="J1:O7" xr:uid="{2FB4BD79-54FB-7D43-BEEE-37F9A827C0DE}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5FF2180F-76F9-A746-8C55-BBB6F0393834}" name="Region" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{D0548A0A-1672-894E-BCDE-D702C6719251}" name="Rep" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{2AF4D54E-D49C-BA48-AAC6-F8060165BB28}" name="Item" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{4DDC914F-CC98-0B4A-98C6-EA049121457C}" name="Units" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{E99A81FC-8139-C141-9352-61D048323D3C}" name="Unit Cost" totalsRowFunction="average" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{75303A0A-2CA3-FC45-B09C-7BEF7FE97225}" name="Total" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{5FF2180F-76F9-A746-8C55-BBB6F0393834}" name="Region" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{D0548A0A-1672-894E-BCDE-D702C6719251}" name="Rep" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{2AF4D54E-D49C-BA48-AAC6-F8060165BB28}" name="Item" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{4DDC914F-CC98-0B4A-98C6-EA049121457C}" name="Units" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{E99A81FC-8139-C141-9352-61D048323D3C}" name="Unit Cost" totalsRowFunction="average" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{75303A0A-2CA3-FC45-B09C-7BEF7FE97225}" name="Total" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Comma">
       <calculatedColumnFormula>Table17[[#This Row],[Units]]*Table17[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1092,11 +1104,28 @@
       <totalsRowFormula>SUBTOTAL(9,Table8[Column3])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DEF2B5E7-1C88-E94A-979A-299DB49B58E3}" name="Column4" totalsRowFunction="sum"/>
-    <tableColumn id="5" xr3:uid="{646CE8D4-3EDF-604D-BB6D-74D5208E9A47}" name="Column5" totalsRowFunction="average" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{646CE8D4-3EDF-604D-BB6D-74D5208E9A47}" name="Column5" totalsRowFunction="average" dataDxfId="1">
       <calculatedColumnFormula>Table8[[#This Row],[Column1]]*Table8[[#This Row],[Column2]]+Table8[[#This Row],[Column3]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{46ABF939-2E75-A94C-B4D8-32D622D17D04}" name="Table9" displayName="Table9" ref="A1:E6" totalsRowCount="1">
+  <autoFilter ref="A1:E5" xr:uid="{46ABF939-2E75-A94C-B4D8-32D622D17D04}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B4C78E4A-C810-8B44-97FD-92554693A24C}" name="Column1" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{869D42C5-61C3-DA4B-8B1D-7C69594DACA4}" name="Hi, 'This" totalsRowFunction="min"/>
+    <tableColumn id="3" xr3:uid="{F425B3AF-69B8-9B49-BA05-2DFA8877087F}" name="#Shame" totalsRowFunction="sum"/>
+    <tableColumn id="4" xr3:uid="{678C209A-B222-C54F-AEDB-ED0775687AB1}" name="[Not me]" totalsRowFunction="count"/>
+    <tableColumn id="5" xr3:uid="{7B266C7B-2FF9-1E48-A132-AB34432EBBB0}" name="Totals []^&amp;*@#$,,&lt;&gt;" totalsRowFunction="custom" dataDxfId="0">
+      <calculatedColumnFormula>SUBTOTAL(109,Table9[[#This Row],[Hi, ''This]:['[Not me']]])</calculatedColumnFormula>
+      <totalsRowFormula>SUM(Table9[Totals '[']^&amp;*@'#$,,&lt;&gt;])</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1988,10 +2017,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D53426B-9C19-C34E-AE5A-A288DFFC9730}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F44"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2016,7 +2045,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -2121,7 +2150,7 @@
         <v>167.44</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>46</v>
       </c>
@@ -2197,8 +2226,8 @@
       <c r="C10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="5">
-        <v>32</v>
+      <c r="D10" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="E10" s="6">
         <v>1.99</v>
@@ -2208,7 +2237,7 @@
         <v>63.68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
@@ -2250,7 +2279,7 @@
         <v>449.1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
@@ -2271,7 +2300,7 @@
         <v>57.71</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
@@ -2292,7 +2321,7 @@
         <v>1619.1899999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
@@ -2334,7 +2363,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -2355,7 +2384,7 @@
         <v>255.84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
@@ -2376,7 +2405,7 @@
         <v>251.72</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
@@ -2398,7 +2427,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>46</v>
       </c>
@@ -2419,7 +2448,7 @@
         <v>299.84999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -2440,7 +2469,7 @@
         <v>479.04</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>48</v>
       </c>
@@ -2461,7 +2490,7 @@
         <v>86.43</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
@@ -2482,7 +2511,7 @@
         <v>1183.26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>48</v>
       </c>
@@ -2503,7 +2532,7 @@
         <v>413.54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
@@ -2524,7 +2553,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -2545,7 +2574,7 @@
         <v>19.96</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>49</v>
       </c>
@@ -2555,18 +2584,22 @@
       <c r="C27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="5">
-        <v>7</v>
+      <c r="D27" s="5" t="b">
+        <f>H27</f>
+        <v>1</v>
       </c>
       <c r="E27" s="6">
         <v>19.989999999999998</v>
       </c>
       <c r="F27" s="7">
         <f>Table16[[#This Row],[Units]]*Table16[[#This Row],[Unit Cost]]</f>
-        <v>139.92999999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>48</v>
       </c>
@@ -2587,7 +2620,7 @@
         <v>249.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
@@ -2608,7 +2641,7 @@
         <v>131.34</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>46</v>
       </c>
@@ -2629,7 +2662,7 @@
         <v>479.04</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>48</v>
       </c>
@@ -2650,7 +2683,7 @@
         <v>68.37</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>48</v>
       </c>
@@ -2692,7 +2725,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>46</v>
       </c>
@@ -2924,50 +2957,88 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D45" t="e">
+      <c r="D45">
         <f>SUBTOTAL(101,Table16[Units])</f>
-        <v>#N/A</v>
+        <v>47.821428571428569</v>
       </c>
       <c r="E45" s="8">
         <f>SUBTOTAL(101,Table16[Unit Cost])</f>
-        <v>20.308604651162792</v>
-      </c>
-      <c r="F45" s="8" t="e">
+        <v>25.146666666666668</v>
+      </c>
+      <c r="F45" s="8">
         <f>SUBTOTAL(109,Table16[Total])</f>
-        <v>#N/A</v>
+        <v>13402.369999999997</v>
       </c>
       <c r="G45" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D46" t="e">
+      <c r="D46">
         <f>SUBTOTAL(1, Table16[Units])</f>
-        <v>#N/A</v>
+        <v>47.821428571428569</v>
       </c>
       <c r="G46" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D47" t="e">
+      <c r="D47">
         <f>SUBTOTAL(4,Table16[Units])</f>
-        <v>#N/A</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D48" t="e">
+      <c r="D48">
         <f>SUBTOTAL(104, Table16[Units])</f>
-        <v>#N/A</v>
+        <v>96</v>
+      </c>
+      <c r="E48">
+        <f>SUBTOTAL(8,Table16[Unit Cost])</f>
+        <v>55.167972492098059</v>
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D49" t="e">
+      <c r="D49">
         <f>SUBTOTAL(109,Table16[#Data])</f>
-        <v>#N/A</v>
+        <v>15495.769999999997</v>
+      </c>
+      <c r="E49">
+        <f>SUBTOTAL(108,Table16[Unit Cost])</f>
+        <v>55.167972492098059</v>
       </c>
       <c r="G49" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D50">
+        <f>SUBTOTAL(2,D6:D45)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D51">
+        <f>SUBTOTAL(102, Table16[[#All],[Units]])</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D52">
+        <f>COUNTA(Table16[[#All],[Units]])</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <f>COUNT(Table16[[#All],[Units]])</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <f>SUBTOTAL(3,Table16[[#All],[Units]])</f>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2980,10 +3051,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C59673F-08B4-F543-8A6A-D28D5C3CA8E0}">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3270,7 +3341,7 @@
         <v>224.55</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -3467,7 +3538,7 @@
         <v>174.65</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
@@ -3543,16 +3614,15 @@
       <c r="C19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="D19" s="5">
+        <v>12</v>
       </c>
       <c r="E19" s="6">
         <v>8.99</v>
       </c>
-      <c r="F19" s="7" t="e">
-        <f>Table17[[#This Row],[Units]]*Table17[[#This Row],[Unit Cost]]</f>
-        <v>#N/A</v>
+      <c r="F19" s="7">
+        <f>Table17[[#This Row],[Units]]*Table17[[#This Row],[Unit Cost]]</f>
+        <v>107.88</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3597,7 +3667,7 @@
         <v>479.04</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>48</v>
       </c>
@@ -3660,7 +3730,7 @@
         <v>413.54</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
@@ -3681,7 +3751,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>46</v>
       </c>
@@ -3744,7 +3814,7 @@
         <v>249.5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>48</v>
       </c>
@@ -3786,7 +3856,7 @@
         <v>479.04</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>48</v>
       </c>
@@ -3870,7 +3940,7 @@
         <v>309.38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>48</v>
       </c>
@@ -3996,7 +4066,7 @@
         <v>1139.4299999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>48</v>
       </c>
@@ -4059,7 +4129,7 @@
         <v>1879.06</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -4084,40 +4154,40 @@
       <c r="A45" t="s">
         <v>6</v>
       </c>
-      <c r="D45" t="e">
+      <c r="D45">
         <f>SUBTOTAL(105,Table17[Units])</f>
-        <v>#N/A</v>
+        <v>0.5</v>
       </c>
       <c r="E45" s="8">
         <f>SUBTOTAL(109,Table17[Unit Cost])</f>
-        <v>721.72</v>
-      </c>
-      <c r="F45" s="8" t="e">
+        <v>854.50000000000011</v>
+      </c>
+      <c r="F45" s="8">
         <f>SUBTOTAL(109,Table17[Total])</f>
-        <v>#N/A</v>
+        <v>17698.495000000003</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D46" t="e">
+      <c r="D46">
         <f>SUBTOTAL(9,Table17[Units])</f>
-        <v>#N/A</v>
+        <v>1820.5</v>
       </c>
       <c r="E46">
         <f>SUBTOTAL(9,Table17[Unit Cost])</f>
-        <v>721.72</v>
+        <v>873.2700000000001</v>
       </c>
       <c r="G46" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D47" t="e">
+      <c r="D47">
         <f>SUBTOTAL(109, Table17[Units])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E47" t="e">
+        <v>1708.5</v>
+      </c>
+      <c r="E47">
         <f>SUBTOTAL(105,Table17[Units])</f>
-        <v>#N/A</v>
+        <v>0.5</v>
       </c>
       <c r="G47" t="s">
         <v>37</v>
@@ -4133,9 +4203,9 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D49" t="e">
+      <c r="D49">
         <f>SUBTOTAL(101.2,Table17[Units])</f>
-        <v>#N/A</v>
+        <v>44.960526315789473</v>
       </c>
       <c r="G49" t="s">
         <v>58</v>
@@ -4144,13 +4214,67 @@
     <row r="51" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E51">
         <f>SUBTOTAL(6,Table17[Unit Cost])</f>
-        <v>7.3394670378456595E+32</v>
+        <v>4.5253473053046947E+37</v>
       </c>
     </row>
     <row r="52" spans="4:7" x14ac:dyDescent="0.2">
       <c r="E52">
         <f>SUBTOTAL(106, Table17[Unit Cost])</f>
-        <v>7.3394670378456595E+32</v>
+        <v>5.6285848990260177E+35</v>
+      </c>
+    </row>
+    <row r="53" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D53">
+        <f>SUBTOTAL(2, Table17[Units])</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D54">
+        <f>SUBTOTAL(102, Table17[Units])</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D55">
+        <f>COUNT(Table17[Units])</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D56">
+        <f>SUBTOTAL(3, Table17[Units])</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D57">
+        <f>SUBTOTAL(103, Table17[Units])</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D58">
+        <f>SUBTOTAL(7, Table17[Units])</f>
+        <v>30.998229689813563</v>
+      </c>
+    </row>
+    <row r="59" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D59">
+        <f>SUBTOTAL(107, Table17[Units])</f>
+        <v>31.453608390717047</v>
+      </c>
+    </row>
+    <row r="60" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D60">
+        <f>SUBTOTAL(8,Table17[#Data])</f>
+        <v>325.68209111039317</v>
+      </c>
+    </row>
+    <row r="61" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D61">
+        <f>SUBTOTAL(108,Table17[#Data])</f>
+        <v>332.38676132436507</v>
       </c>
     </row>
   </sheetData>
@@ -4166,7 +4290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B23473F-5DA6-0940-893D-89F02152A971}">
   <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -4301,4 +4425,148 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16AB3B-025F-D442-B8C0-62CD2364AA9F}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <f>SUBTOTAL(109,Table9[[#This Row],[Hi, ''This]:['[Not me']]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <f>SUBTOTAL(109,Table9[[#This Row],[Hi, ''This]:['[Not me']]])</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <f>SUBTOTAL(109,Table9[[#This Row],[Hi, ''This]:['[Not me']]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <f>SUBTOTAL(109,Table9[[#This Row],[Hi, ''This]:['[Not me']]])</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>SUBTOTAL(105,Table9[Hi, ''This])</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f>SUBTOTAL(109,Table9['#Shame])</f>
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <f>SUBTOTAL(103,Table9['[Not me']])</f>
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f>SUM(Table9[Totals '[']^&amp;*@'#$,,&lt;&gt;])</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f>SUBTOTAL(10,B2:E3)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f>SUBTOTAL(11,Table9[#Data])</f>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f>SUBTOTAL(110,A2:E8)</f>
+        <v>60.266666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f>SUBTOTAL(111,A2:E8)</f>
+        <v>54.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
UPDATE:[Calc]: Adds some information functions (7) (#317)
ISREF, ISODD, ISEVEN, ERROR.TYPE, ISFORMULA, TYPE, SHEET

Also adds #NULL! error type
</commit_message>
<xml_diff>
--- a/packages/calc/equalto_xlsx/tests/calc_test_no_export/tables.xlsx
+++ b/packages/calc/equalto_xlsx/tests/calc_test_no_export/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Library/CloudStorage/Dropbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C75E367-1D12-644E-9BDE-F8C50425E666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295E10DD-5E3F-914A-B04F-FE53893A365E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="2460" windowWidth="28040" windowHeight="17440" activeTab="7" xr2:uid="{234D3629-A973-D04E-93AE-20E06D5B5DDB}"/>
+    <workbookView xWindow="4200" yWindow="2460" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{234D3629-A973-D04E-93AE-20E06D5B5DDB}"/>
   </bookViews>
   <sheets>
     <sheet name="WithHeaders" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,12 @@
     <sheet name="Functions Hidden" sheetId="6" r:id="rId6"/>
     <sheet name="No Headers" sheetId="7" r:id="rId7"/>
     <sheet name="Escape" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="Fancy">Sheet2!$B$11</definedName>
+    <definedName name="Hello" localSheetId="4">'Functions Filters'!$L$4</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="74">
   <si>
     <t>Jan</t>
   </si>
@@ -250,6 +255,21 @@
   </si>
   <si>
     <t>Hi, 'This</t>
+  </si>
+  <si>
+    <t>Where sheets are</t>
+  </si>
+  <si>
+    <t>&lt;= Table 1</t>
+  </si>
+  <si>
+    <t>Hi I'm a defined name</t>
+  </si>
+  <si>
+    <t>Defined names</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
 </sst>
 </file>
@@ -1426,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559AFA5D-3006-5748-AD42-29115B1892A2}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1574,16 +1594,22 @@
         <v>JanFebMarAprDecYear</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F17">
         <f>SUM(Table1[#Data])</f>
         <v>274</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F18">
         <f>SUM(Table1[#All])</f>
         <v>538</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f ca="1">_xlfn.SHEET()</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1597,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04143B8D-987F-9746-B127-5D8AA7B9D7F0}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1667,6 +1693,11 @@
       <c r="F4" t="e">
         <f>SUM(Table2[#Totals])</f>
         <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2017,15 +2048,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D53426B-9C19-C34E-AE5A-A288DFFC9730}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -2045,7 +2076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -2066,7 +2097,7 @@
         <v>189.05</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
@@ -2087,7 +2118,7 @@
         <v>999.49999999999989</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>48</v>
       </c>
@@ -2107,8 +2138,11 @@
         <f>Table16[[#This Row],[Units]]*Table16[[#This Row],[Unit Cost]]</f>
         <v>179.64000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>48</v>
       </c>
@@ -2129,7 +2163,7 @@
         <v>539.7299999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
@@ -2150,7 +2184,7 @@
         <v>167.44</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>46</v>
       </c>
@@ -2171,7 +2205,7 @@
         <v>224.55</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
@@ -2192,7 +2226,7 @@
         <v>45.77</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
@@ -2216,7 +2250,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
@@ -2237,7 +2271,7 @@
         <v>63.68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
@@ -2258,7 +2292,7 @@
         <v>539.4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>48</v>
       </c>
@@ -2279,7 +2313,7 @@
         <v>449.1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
@@ -2300,7 +2334,7 @@
         <v>57.71</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>46</v>
       </c>
@@ -2321,7 +2355,7 @@
         <v>1619.1899999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>46</v>
       </c>
@@ -2342,7 +2376,7 @@
         <v>174.65</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>48</v>
       </c>
@@ -3054,7 +3088,7 @@
   <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3898,7 +3932,7 @@
         <v>719.2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>48</v>
       </c>
@@ -3919,7 +3953,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>46</v>
       </c>
@@ -3940,7 +3974,7 @@
         <v>309.38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>48</v>
       </c>
@@ -3961,7 +3995,7 @@
         <v>686.95</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>48</v>
       </c>
@@ -3982,7 +4016,7 @@
         <v>1005.9</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>49</v>
       </c>
@@ -4003,7 +4037,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -4023,8 +4057,12 @@
         <f>Table17[[#This Row],[Units]]*Table17[[#This Row],[Unit Cost]]</f>
         <v>9.0300000000000011</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <f ca="1">_xlfn.SHEET()</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>49</v>
       </c>
@@ -4045,7 +4083,7 @@
         <v>151.24</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>49</v>
       </c>
@@ -4066,7 +4104,7 @@
         <v>1139.4299999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>48</v>
       </c>
@@ -4087,7 +4125,7 @@
         <v>18.060000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>48</v>
       </c>
@@ -4108,7 +4146,7 @@
         <v>54.89</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>48</v>
       </c>
@@ -4129,7 +4167,7 @@
         <v>1879.06</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>48</v>
       </c>
@@ -4150,7 +4188,7 @@
         <v>139.72</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -4167,7 +4205,7 @@
         <v>17698.495000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D46">
         <f>SUBTOTAL(9,Table17[Units])</f>
         <v>1820.5</v>
@@ -4180,7 +4218,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D47">
         <f>SUBTOTAL(109, Table17[Units])</f>
         <v>1708.5</v>
@@ -4193,7 +4231,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D48" t="e">
         <f>SUBTOTAL(205, Table17[Units])</f>
         <v>#VALUE!</v>
@@ -4290,8 +4328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B23473F-5DA6-0940-893D-89F02152A971}">
   <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4429,10 +4467,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16AB3B-025F-D442-B8C0-62CD2364AA9F}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4563,10 +4601,88 @@
         <v>54.24</v>
       </c>
     </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <f ca="1">_xlfn.SHEET("Filters")</f>
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11439324-B322-A545-9A5B-8F828FE81105}">
+  <dimension ref="A4:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f ca="1">_xlfn.SHEET(Table1[])</f>
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <f ca="1">_xlfn.SHEET("Hidden")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f ca="1">_xlfn.SHEET(Table2[])</f>
+        <v>2</v>
+      </c>
+      <c r="D6" t="e">
+        <f ca="1">_xlfn.SHEET(1)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f ca="1">_xlfn.SHEET(Table3[])</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f ca="1">_xlfn.SHEET(Table4[])</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f ca="1">_xlfn.SHEET(Fancy)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="e">
+        <f ca="1">_xlfn.SHEET(Hello)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>